<commit_message>
+ Lord Of The Rings Taverns
</commit_message>
<xml_diff>
--- a/Dim/FictionalCompanyNames_ v0-00-001.xlsx
+++ b/Dim/FictionalCompanyNames_ v0-00-001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Datasets\Dim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9918DC-95F8-476D-BFAE-A6122FB52274}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51917B7F-49AF-4223-8EA0-28027FFCB502}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="0" windowWidth="19560" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="681">
   <si>
     <t>Company Name</t>
   </si>
@@ -2048,6 +2048,36 @@
   </si>
   <si>
     <t>The Never Ending Story</t>
+  </si>
+  <si>
+    <t>The Prancing Pony</t>
+  </si>
+  <si>
+    <t>Restaurant, Nightclub, Hotel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bree </t>
+  </si>
+  <si>
+    <t>The Lord Of The Rings</t>
+  </si>
+  <si>
+    <t>Barliman Butterbur</t>
+  </si>
+  <si>
+    <t>Aragorn</t>
+  </si>
+  <si>
+    <t>The Green Dragon Inn</t>
+  </si>
+  <si>
+    <t>The Shire</t>
+  </si>
+  <si>
+    <t>Rosie Cotton</t>
+  </si>
+  <si>
+    <t>Samwise Gamgee</t>
   </si>
 </sst>
 </file>
@@ -2675,10 +2705,10 @@
   <dimension ref="A1:AC1005"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="A173" sqref="A173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9270,25 +9300,25 @@
     </row>
     <row r="151" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
-        <v>215</v>
+        <v>677</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>271</v>
+        <v>672</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>272</v>
+        <v>678</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="E151" s="3" t="s">
-        <v>354</v>
+        <v>674</v>
+      </c>
+      <c r="E151" s="4" t="s">
+        <v>442</v>
       </c>
       <c r="F151" s="4" t="s">
-        <v>217</v>
+        <v>679</v>
       </c>
       <c r="G151" s="4" t="s">
-        <v>216</v>
+        <v>680</v>
       </c>
       <c r="H151" s="4"/>
       <c r="I151" s="4"/>
@@ -9315,24 +9345,26 @@
     </row>
     <row r="152" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
-        <v>559</v>
+        <v>215</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>560</v>
+        <v>271</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>561</v>
+        <v>272</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>562</v>
-      </c>
-      <c r="E152" s="4" t="s">
-        <v>329</v>
+        <v>216</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>354</v>
       </c>
       <c r="F152" s="4" t="s">
-        <v>563</v>
-      </c>
-      <c r="G152" s="4"/>
+        <v>217</v>
+      </c>
+      <c r="G152" s="4" t="s">
+        <v>216</v>
+      </c>
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
       <c r="J152" s="4"/>
@@ -9357,23 +9389,23 @@
       <c r="AC152" s="4"/>
     </row>
     <row r="153" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A153" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="C153" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D153" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E153" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="F153" s="3" t="s">
-        <v>474</v>
+      <c r="A153" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="D153" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="E153" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="F153" s="4" t="s">
+        <v>563</v>
       </c>
       <c r="G153" s="4"/>
       <c r="H153" s="4"/>
@@ -9401,24 +9433,26 @@
     </row>
     <row r="154" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
-        <v>397</v>
+        <v>671</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>311</v>
+        <v>672</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>398</v>
+        <v>673</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>399</v>
+        <v>674</v>
       </c>
       <c r="E154" s="4" t="s">
-        <v>342</v>
+        <v>442</v>
       </c>
       <c r="F154" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="G154" s="4"/>
+        <v>675</v>
+      </c>
+      <c r="G154" s="4" t="s">
+        <v>676</v>
+      </c>
       <c r="H154" s="4"/>
       <c r="I154" s="4"/>
       <c r="J154" s="4"/>
@@ -9443,27 +9477,25 @@
       <c r="AC154" s="4"/>
     </row>
     <row r="155" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A155" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="B155" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="C155" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="D155" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="E155" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="F155" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="G155" s="4" t="s">
-        <v>341</v>
-      </c>
+      <c r="A155" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E155" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="G155" s="4"/>
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>
       <c r="J155" s="4"/>
@@ -9489,22 +9521,22 @@
     </row>
     <row r="156" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
-        <v>644</v>
+        <v>397</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>645</v>
-      </c>
-      <c r="C156" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D156" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E156" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C156" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="D156" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="E156" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="F156" s="3" t="s">
-        <v>57</v>
+      <c r="F156" s="4" t="s">
+        <v>400</v>
       </c>
       <c r="G156" s="4"/>
       <c r="H156" s="4"/>
@@ -9531,25 +9563,27 @@
       <c r="AC156" s="4"/>
     </row>
     <row r="157" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A157" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B157" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="C157" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D157" s="3" t="s">
-        <v>154</v>
+      <c r="A157" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D157" s="4" t="s">
+        <v>336</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="F157" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G157" s="4"/>
+        <v>322</v>
+      </c>
+      <c r="F157" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="G157" s="4" t="s">
+        <v>341</v>
+      </c>
       <c r="H157" s="4"/>
       <c r="I157" s="4"/>
       <c r="J157" s="4"/>
@@ -9575,26 +9609,24 @@
     </row>
     <row r="158" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
-        <v>290</v>
+        <v>644</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="C158" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="D158" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="E158" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="F158" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="G158" s="4" t="s">
-        <v>231</v>
-      </c>
+        <v>645</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G158" s="4"/>
       <c r="H158" s="4"/>
       <c r="I158" s="4"/>
       <c r="J158" s="4"/>
@@ -9620,26 +9652,24 @@
     </row>
     <row r="159" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
-        <v>251</v>
+        <v>130</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>250</v>
+        <v>279</v>
       </c>
       <c r="C159" s="3" t="s">
         <v>261</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>42</v>
+        <v>154</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>329</v>
+        <v>355</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="G159" s="4" t="s">
-        <v>181</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="G159" s="4"/>
       <c r="H159" s="4"/>
       <c r="I159" s="4"/>
       <c r="J159" s="4"/>
@@ -9665,25 +9695,25 @@
     </row>
     <row r="160" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
-        <v>410</v>
+        <v>290</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>411</v>
+        <v>292</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>261</v>
+        <v>291</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>15</v>
+        <v>229</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="F160" s="4" t="s">
-        <v>412</v>
+        <v>230</v>
       </c>
       <c r="G160" s="4" t="s">
-        <v>413</v>
+        <v>231</v>
       </c>
       <c r="H160" s="4"/>
       <c r="I160" s="4"/>
@@ -9709,25 +9739,27 @@
       <c r="AC160" s="4"/>
     </row>
     <row r="161" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A161" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="B161" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="C161" s="4" t="s">
+      <c r="A161" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C161" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D161" s="4" t="s">
-        <v>454</v>
+      <c r="D161" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E161" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="F161" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="G161" s="4"/>
+      <c r="F161" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G161" s="4" t="s">
+        <v>181</v>
+      </c>
       <c r="H161" s="4"/>
       <c r="I161" s="4"/>
       <c r="J161" s="4"/>
@@ -9752,25 +9784,27 @@
       <c r="AC161" s="4"/>
     </row>
     <row r="162" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A162" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>638</v>
-      </c>
-      <c r="C162" s="3" t="s">
+      <c r="A162" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="C162" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D162" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E162" s="3" t="s">
+      <c r="D162" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E162" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="F162" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="G162" s="4"/>
+      <c r="F162" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="G162" s="4" t="s">
+        <v>413</v>
+      </c>
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
       <c r="J162" s="4"/>
@@ -9796,22 +9830,22 @@
     </row>
     <row r="163" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
-        <v>232</v>
+        <v>452</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>505</v>
+        <v>453</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>506</v>
+        <v>261</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>233</v>
+        <v>454</v>
       </c>
       <c r="E163" s="4" t="s">
         <v>329</v>
       </c>
       <c r="F163" s="4" t="s">
-        <v>234</v>
+        <v>455</v>
       </c>
       <c r="G163" s="4"/>
       <c r="H163" s="4"/>
@@ -9838,27 +9872,25 @@
       <c r="AC163" s="4"/>
     </row>
     <row r="164" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A164" s="4" t="s">
-        <v>481</v>
-      </c>
-      <c r="B164" s="4" t="s">
-        <v>480</v>
-      </c>
-      <c r="C164" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="D164" s="4" t="s">
-        <v>482</v>
-      </c>
-      <c r="E164" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="F164" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="G164" s="4" t="s">
-        <v>484</v>
-      </c>
+      <c r="A164" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G164" s="4"/>
       <c r="H164" s="4"/>
       <c r="I164" s="4"/>
       <c r="J164" s="4"/>
@@ -9884,22 +9916,22 @@
     </row>
     <row r="165" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>279</v>
+        <v>232</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>505</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>261</v>
+        <v>506</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>154</v>
+        <v>233</v>
       </c>
       <c r="E165" s="4" t="s">
-        <v>355</v>
+        <v>329</v>
       </c>
       <c r="F165" s="4" t="s">
-        <v>281</v>
+        <v>234</v>
       </c>
       <c r="G165" s="4"/>
       <c r="H165" s="4"/>
@@ -9926,26 +9958,26 @@
       <c r="AC165" s="4"/>
     </row>
     <row r="166" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A166" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B166" s="3" t="s">
+      <c r="A166" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="B166" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="C166" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D166" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="E166" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="F166" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G166" s="3" t="s">
-        <v>20</v>
+      <c r="C166" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="E166" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="F166" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="G166" s="4" t="s">
+        <v>484</v>
       </c>
       <c r="H166" s="4"/>
       <c r="I166" s="4"/>
@@ -9972,22 +10004,22 @@
     </row>
     <row r="167" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
-        <v>534</v>
-      </c>
-      <c r="B167" s="4" t="s">
-        <v>535</v>
+        <v>280</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>279</v>
       </c>
       <c r="C167" s="4" t="s">
         <v>261</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>454</v>
+        <v>154</v>
       </c>
       <c r="E167" s="4" t="s">
-        <v>329</v>
+        <v>355</v>
       </c>
       <c r="F167" s="4" t="s">
-        <v>536</v>
+        <v>281</v>
       </c>
       <c r="G167" s="4"/>
       <c r="H167" s="4"/>
@@ -10015,25 +10047,25 @@
     </row>
     <row r="168" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
-        <v>148</v>
+        <v>214</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>637</v>
+        <v>480</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>447</v>
+        <v>261</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>135</v>
+        <v>247</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>355</v>
+        <v>466</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>149</v>
+        <v>19</v>
       </c>
       <c r="G168" s="3" t="s">
-        <v>136</v>
+        <v>20</v>
       </c>
       <c r="H168" s="4"/>
       <c r="I168" s="4"/>
@@ -10060,22 +10092,22 @@
     </row>
     <row r="169" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
-        <v>633</v>
+        <v>534</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>634</v>
+        <v>535</v>
       </c>
       <c r="C169" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D169" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E169" s="3" t="s">
-        <v>342</v>
+      <c r="D169" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="E169" s="4" t="s">
+        <v>329</v>
       </c>
       <c r="F169" s="4" t="s">
-        <v>636</v>
+        <v>536</v>
       </c>
       <c r="G169" s="4"/>
       <c r="H169" s="4"/>
@@ -10102,26 +10134,26 @@
       <c r="AC169" s="4"/>
     </row>
     <row r="170" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A170" s="4" t="s">
-        <v>606</v>
-      </c>
-      <c r="B170" s="4" t="s">
-        <v>415</v>
-      </c>
-      <c r="C170" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="D170" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="E170" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="F170" s="4" t="s">
-        <v>605</v>
-      </c>
-      <c r="G170" s="4" t="s">
-        <v>604</v>
+      <c r="A170" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G170" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="H170" s="4"/>
       <c r="I170" s="4"/>
@@ -10148,22 +10180,22 @@
     </row>
     <row r="171" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
-        <v>268</v>
+        <v>633</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>270</v>
+        <v>634</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="D171" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E171" s="4" t="s">
-        <v>355</v>
+        <v>261</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>342</v>
       </c>
       <c r="F171" s="4" t="s">
-        <v>208</v>
+        <v>636</v>
       </c>
       <c r="G171" s="4"/>
       <c r="H171" s="4"/>
@@ -10190,13 +10222,27 @@
       <c r="AC171" s="4"/>
     </row>
     <row r="172" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A172" s="4"/>
-      <c r="B172" s="4"/>
-      <c r="C172" s="4"/>
-      <c r="D172" s="4"/>
-      <c r="E172" s="4"/>
-      <c r="F172" s="4"/>
-      <c r="G172" s="4"/>
+      <c r="A172" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="C172" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D172" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="E172" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="F172" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="G172" s="4" t="s">
+        <v>604</v>
+      </c>
       <c r="H172" s="4"/>
       <c r="I172" s="4"/>
       <c r="J172" s="4"/>
@@ -10221,12 +10267,24 @@
       <c r="AC172" s="4"/>
     </row>
     <row r="173" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A173" s="4"/>
-      <c r="B173" s="4"/>
-      <c r="C173" s="4"/>
-      <c r="D173" s="4"/>
-      <c r="E173" s="4"/>
-      <c r="F173" s="4"/>
+      <c r="A173" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C173" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D173" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E173" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="F173" s="4" t="s">
+        <v>208</v>
+      </c>
       <c r="G173" s="4"/>
       <c r="H173" s="4"/>
       <c r="I173" s="4"/>

</xml_diff>

<commit_message>
+ Scoops Ahoy (Stranger Things)
</commit_message>
<xml_diff>
--- a/Dim/FictionalCompanyNames_ v0-00-001.xlsx
+++ b/Dim/FictionalCompanyNames_ v0-00-001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Datasets\Dim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51917B7F-49AF-4223-8EA0-28027FFCB502}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE74EB5-302B-4D8A-853E-C7BD5ADF0993}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="0" windowWidth="19560" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="686">
   <si>
     <t>Company Name</t>
   </si>
@@ -2078,6 +2078,21 @@
   </si>
   <si>
     <t>Samwise Gamgee</t>
+  </si>
+  <si>
+    <t>Scoops Ahoy</t>
+  </si>
+  <si>
+    <t>Ice Cream Parlor</t>
+  </si>
+  <si>
+    <t>Stranger Things</t>
+  </si>
+  <si>
+    <t>Robin Buckley</t>
+  </si>
+  <si>
+    <t>Steve Harrington</t>
   </si>
 </sst>
 </file>
@@ -2705,10 +2720,10 @@
   <dimension ref="A1:AC1005"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B119" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A173" sqref="A173"/>
+      <selection pane="bottomRight" activeCell="A174" sqref="A174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8642,26 +8657,26 @@
       <c r="AC135" s="4"/>
     </row>
     <row r="136" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A136" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="C136" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="D136" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E136" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="F136" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G136" s="3" t="s">
-        <v>114</v>
+      <c r="A136" s="4" t="s">
+        <v>681</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="E136" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="F136" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="G136" s="4" t="s">
+        <v>685</v>
       </c>
       <c r="H136" s="4"/>
       <c r="I136" s="4"/>
@@ -8687,25 +8702,27 @@
       <c r="AC136" s="4"/>
     </row>
     <row r="137" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A137" s="4" t="s">
-        <v>595</v>
+      <c r="A137" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>594</v>
+        <v>445</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>261</v>
+        <v>444</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E137" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="F137" s="4" t="s">
-        <v>596</v>
-      </c>
-      <c r="G137" s="4"/>
+        <v>112</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G137" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="H137" s="4"/>
       <c r="I137" s="4"/>
       <c r="J137" s="4"/>
@@ -8731,22 +8748,22 @@
     </row>
     <row r="138" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
-        <v>576</v>
-      </c>
-      <c r="B138" s="4" t="s">
-        <v>577</v>
-      </c>
-      <c r="C138" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="C138" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D138" s="4" t="s">
-        <v>220</v>
+      <c r="D138" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="E138" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F138" s="4" t="s">
-        <v>578</v>
+        <v>596</v>
       </c>
       <c r="G138" s="4"/>
       <c r="H138" s="4"/>
@@ -8773,24 +8790,25 @@
       <c r="AC138" s="4"/>
     </row>
     <row r="139" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A139" s="3" t="s">
-        <v>470</v>
+      <c r="A139" s="4" t="s">
+        <v>576</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>590</v>
-      </c>
-      <c r="C139" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="C139" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D139" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="E139" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="F139" s="3" t="s">
-        <v>471</v>
-      </c>
+      <c r="D139" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="E139" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="F139" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="G139" s="4"/>
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
       <c r="J139" s="4"/>
@@ -8815,26 +8833,23 @@
       <c r="AC139" s="4"/>
     </row>
     <row r="140" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A140" s="4" t="s">
-        <v>366</v>
+      <c r="A140" s="3" t="s">
+        <v>470</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="C140" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="D140" s="4" t="s">
-        <v>490</v>
-      </c>
-      <c r="E140" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="F140" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="G140" s="4" t="s">
-        <v>370</v>
+        <v>590</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>471</v>
       </c>
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
@@ -8860,26 +8875,26 @@
       <c r="AC140" s="4"/>
     </row>
     <row r="141" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A141" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D141" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E141" s="3" t="s">
+      <c r="A141" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="D141" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="E141" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="F141" s="3" t="s">
-        <v>2</v>
+      <c r="F141" s="4" t="s">
+        <v>369</v>
       </c>
       <c r="G141" s="4" t="s">
-        <v>183</v>
+        <v>370</v>
       </c>
       <c r="H141" s="4"/>
       <c r="I141" s="4"/>
@@ -8906,25 +8921,25 @@
     </row>
     <row r="142" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>485</v>
+        <v>304</v>
       </c>
       <c r="C142" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D142" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="E142" s="4" t="s">
-        <v>466</v>
+      <c r="D142" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>354</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="G142" s="4" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="H142" s="4"/>
       <c r="I142" s="4"/>
@@ -8951,24 +8966,26 @@
     </row>
     <row r="143" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>327</v>
+        <v>485</v>
       </c>
       <c r="C143" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D143" s="3" t="s">
-        <v>117</v>
+      <c r="D143" s="4" t="s">
+        <v>248</v>
       </c>
       <c r="E143" s="4" t="s">
-        <v>342</v>
+        <v>466</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G143" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="G143" s="4" t="s">
+        <v>159</v>
+      </c>
       <c r="H143" s="4"/>
       <c r="I143" s="4"/>
       <c r="J143" s="4"/>
@@ -8994,22 +9011,22 @@
     </row>
     <row r="144" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B144" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="C144" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C144" s="3" t="s">
         <v>261</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G144" s="4"/>
       <c r="H144" s="4"/>
@@ -9036,27 +9053,25 @@
       <c r="AC144" s="4"/>
     </row>
     <row r="145" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A145" s="4" t="s">
-        <v>238</v>
+      <c r="A145" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>504</v>
+        <v>265</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="D145" s="4" t="s">
-        <v>233</v>
+        <v>261</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="E145" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="F145" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="G145" s="4" t="s">
-        <v>240</v>
-      </c>
+        <v>355</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G145" s="4"/>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
       <c r="J145" s="4"/>
@@ -9082,24 +9097,26 @@
     </row>
     <row r="146" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
-        <v>510</v>
+        <v>238</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>459</v>
+        <v>504</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>511</v>
-      </c>
-      <c r="D146" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D146" s="4" t="s">
         <v>233</v>
       </c>
       <c r="E146" s="4" t="s">
         <v>329</v>
       </c>
       <c r="F146" s="4" t="s">
-        <v>512</v>
-      </c>
-      <c r="G146" s="4"/>
+        <v>239</v>
+      </c>
+      <c r="G146" s="4" t="s">
+        <v>240</v>
+      </c>
       <c r="H146" s="4"/>
       <c r="I146" s="4"/>
       <c r="J146" s="4"/>
@@ -9125,26 +9142,24 @@
     </row>
     <row r="147" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
-        <v>151</v>
+        <v>510</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>265</v>
+        <v>459</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="D147" s="4" t="s">
-        <v>22</v>
+        <v>511</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>233</v>
       </c>
       <c r="E147" s="4" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="F147" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="G147" s="4" t="s">
-        <v>153</v>
-      </c>
+        <v>512</v>
+      </c>
+      <c r="G147" s="4"/>
       <c r="H147" s="4"/>
       <c r="I147" s="4"/>
       <c r="J147" s="4"/>
@@ -9170,25 +9185,25 @@
     </row>
     <row r="148" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
-        <v>339</v>
+        <v>151</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>343</v>
+        <v>265</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>319</v>
+        <v>261</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>336</v>
+        <v>22</v>
       </c>
       <c r="E148" s="4" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="F148" s="4" t="s">
-        <v>337</v>
+        <v>152</v>
       </c>
       <c r="G148" s="4" t="s">
-        <v>338</v>
+        <v>153</v>
       </c>
       <c r="H148" s="4"/>
       <c r="I148" s="4"/>
@@ -9214,23 +9229,26 @@
       <c r="AC148" s="4"/>
     </row>
     <row r="149" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A149" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>656</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D149" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E149" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="F149" s="3" t="s">
-        <v>657</v>
+      <c r="A149" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D149" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="E149" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="F149" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="G149" s="4" t="s">
+        <v>338</v>
       </c>
       <c r="H149" s="4"/>
       <c r="I149" s="4"/>
@@ -9257,24 +9275,23 @@
     </row>
     <row r="150" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>641</v>
+        <v>656</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>261</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>342</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G150" s="4"/>
+        <v>657</v>
+      </c>
       <c r="H150" s="4"/>
       <c r="I150" s="4"/>
       <c r="J150" s="4"/>
@@ -9299,27 +9316,25 @@
       <c r="AC150" s="4"/>
     </row>
     <row r="151" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A151" s="4" t="s">
-        <v>677</v>
-      </c>
-      <c r="B151" s="4" t="s">
-        <v>672</v>
-      </c>
-      <c r="C151" s="4" t="s">
-        <v>678</v>
-      </c>
-      <c r="D151" s="4" t="s">
-        <v>674</v>
-      </c>
-      <c r="E151" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="F151" s="4" t="s">
-        <v>679</v>
-      </c>
-      <c r="G151" s="4" t="s">
-        <v>680</v>
-      </c>
+      <c r="A151" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G151" s="4"/>
       <c r="H151" s="4"/>
       <c r="I151" s="4"/>
       <c r="J151" s="4"/>
@@ -9345,25 +9360,25 @@
     </row>
     <row r="152" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
-        <v>215</v>
+        <v>677</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>271</v>
+        <v>672</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>272</v>
+        <v>678</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="E152" s="3" t="s">
-        <v>354</v>
+        <v>674</v>
+      </c>
+      <c r="E152" s="4" t="s">
+        <v>442</v>
       </c>
       <c r="F152" s="4" t="s">
-        <v>217</v>
+        <v>679</v>
       </c>
       <c r="G152" s="4" t="s">
-        <v>216</v>
+        <v>680</v>
       </c>
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
@@ -9390,24 +9405,26 @@
     </row>
     <row r="153" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
-        <v>559</v>
+        <v>215</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>560</v>
+        <v>271</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>561</v>
+        <v>272</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>562</v>
-      </c>
-      <c r="E153" s="4" t="s">
-        <v>329</v>
+        <v>216</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>354</v>
       </c>
       <c r="F153" s="4" t="s">
-        <v>563</v>
-      </c>
-      <c r="G153" s="4"/>
+        <v>217</v>
+      </c>
+      <c r="G153" s="4" t="s">
+        <v>216</v>
+      </c>
       <c r="H153" s="4"/>
       <c r="I153" s="4"/>
       <c r="J153" s="4"/>
@@ -9433,26 +9450,24 @@
     </row>
     <row r="154" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
-        <v>671</v>
+        <v>559</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>672</v>
+        <v>560</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>673</v>
+        <v>561</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>674</v>
+        <v>562</v>
       </c>
       <c r="E154" s="4" t="s">
-        <v>442</v>
+        <v>329</v>
       </c>
       <c r="F154" s="4" t="s">
-        <v>675</v>
-      </c>
-      <c r="G154" s="4" t="s">
-        <v>676</v>
-      </c>
+        <v>563</v>
+      </c>
+      <c r="G154" s="4"/>
       <c r="H154" s="4"/>
       <c r="I154" s="4"/>
       <c r="J154" s="4"/>
@@ -9477,25 +9492,27 @@
       <c r="AC154" s="4"/>
     </row>
     <row r="155" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A155" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="C155" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D155" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E155" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="F155" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="G155" s="4"/>
+      <c r="A155" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>672</v>
+      </c>
+      <c r="C155" s="4" t="s">
+        <v>673</v>
+      </c>
+      <c r="D155" s="4" t="s">
+        <v>674</v>
+      </c>
+      <c r="E155" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="F155" s="4" t="s">
+        <v>675</v>
+      </c>
+      <c r="G155" s="4" t="s">
+        <v>676</v>
+      </c>
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>
       <c r="J155" s="4"/>
@@ -9520,23 +9537,23 @@
       <c r="AC155" s="4"/>
     </row>
     <row r="156" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A156" s="4" t="s">
-        <v>397</v>
-      </c>
-      <c r="B156" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="C156" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="D156" s="4" t="s">
-        <v>399</v>
-      </c>
-      <c r="E156" s="4" t="s">
+      <c r="A156" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E156" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="F156" s="4" t="s">
-        <v>400</v>
+      <c r="F156" s="3" t="s">
+        <v>474</v>
       </c>
       <c r="G156" s="4"/>
       <c r="H156" s="4"/>
@@ -9564,26 +9581,24 @@
     </row>
     <row r="157" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
-        <v>334</v>
+        <v>397</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>319</v>
+        <v>398</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>336</v>
+        <v>399</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="F157" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="G157" s="4" t="s">
-        <v>341</v>
-      </c>
+        <v>400</v>
+      </c>
+      <c r="G157" s="4"/>
       <c r="H157" s="4"/>
       <c r="I157" s="4"/>
       <c r="J157" s="4"/>
@@ -9609,24 +9624,26 @@
     </row>
     <row r="158" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
-        <v>644</v>
+        <v>334</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>645</v>
-      </c>
-      <c r="C158" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D158" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E158" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="F158" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G158" s="4"/>
+        <v>335</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D158" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="E158" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="F158" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="G158" s="4" t="s">
+        <v>341</v>
+      </c>
       <c r="H158" s="4"/>
       <c r="I158" s="4"/>
       <c r="J158" s="4"/>
@@ -9651,23 +9668,23 @@
       <c r="AC158" s="4"/>
     </row>
     <row r="159" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A159" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>279</v>
+      <c r="A159" s="4" t="s">
+        <v>644</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>645</v>
       </c>
       <c r="C159" s="3" t="s">
         <v>261</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E159" s="4" t="s">
-        <v>355</v>
+        <v>56</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>342</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>131</v>
+        <v>57</v>
       </c>
       <c r="G159" s="4"/>
       <c r="H159" s="4"/>
@@ -9694,27 +9711,25 @@
       <c r="AC159" s="4"/>
     </row>
     <row r="160" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A160" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="B160" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="C160" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="D160" s="4" t="s">
-        <v>229</v>
+      <c r="A160" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="F160" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="G160" s="4" t="s">
-        <v>231</v>
-      </c>
+        <v>355</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G160" s="4"/>
       <c r="H160" s="4"/>
       <c r="I160" s="4"/>
       <c r="J160" s="4"/>
@@ -9739,26 +9754,26 @@
       <c r="AC160" s="4"/>
     </row>
     <row r="161" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A161" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D161" s="3" t="s">
-        <v>42</v>
+      <c r="A161" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C161" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D161" s="4" t="s">
+        <v>229</v>
       </c>
       <c r="E161" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="F161" s="3" t="s">
-        <v>180</v>
+      <c r="F161" s="4" t="s">
+        <v>230</v>
       </c>
       <c r="G161" s="4" t="s">
-        <v>181</v>
+        <v>231</v>
       </c>
       <c r="H161" s="4"/>
       <c r="I161" s="4"/>
@@ -9784,26 +9799,26 @@
       <c r="AC161" s="4"/>
     </row>
     <row r="162" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A162" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="B162" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="C162" s="4" t="s">
+      <c r="A162" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C162" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D162" s="4" t="s">
-        <v>15</v>
+      <c r="D162" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E162" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="F162" s="4" t="s">
-        <v>412</v>
+        <v>329</v>
+      </c>
+      <c r="F162" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="G162" s="4" t="s">
-        <v>413</v>
+        <v>181</v>
       </c>
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
@@ -9830,24 +9845,26 @@
     </row>
     <row r="163" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
-        <v>452</v>
+        <v>410</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>453</v>
+        <v>411</v>
       </c>
       <c r="C163" s="4" t="s">
         <v>261</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>454</v>
+        <v>15</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="F163" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="G163" s="4"/>
+        <v>412</v>
+      </c>
+      <c r="G163" s="4" t="s">
+        <v>413</v>
+      </c>
       <c r="H163" s="4"/>
       <c r="I163" s="4"/>
       <c r="J163" s="4"/>
@@ -9872,23 +9889,23 @@
       <c r="AC163" s="4"/>
     </row>
     <row r="164" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A164" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>638</v>
-      </c>
-      <c r="C164" s="3" t="s">
+      <c r="A164" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="C164" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D164" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E164" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="F164" s="3" t="s">
-        <v>134</v>
+      <c r="D164" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="E164" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="F164" s="4" t="s">
+        <v>455</v>
       </c>
       <c r="G164" s="4"/>
       <c r="H164" s="4"/>
@@ -9915,23 +9932,23 @@
       <c r="AC164" s="4"/>
     </row>
     <row r="165" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A165" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="B165" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="C165" s="4" t="s">
-        <v>506</v>
-      </c>
-      <c r="D165" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="E165" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="F165" s="4" t="s">
-        <v>234</v>
+      <c r="A165" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="G165" s="4"/>
       <c r="H165" s="4"/>
@@ -9959,26 +9976,24 @@
     </row>
     <row r="166" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
-        <v>481</v>
+        <v>232</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>480</v>
+        <v>505</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>269</v>
+        <v>506</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>482</v>
+        <v>233</v>
       </c>
       <c r="E166" s="4" t="s">
-        <v>355</v>
+        <v>329</v>
       </c>
       <c r="F166" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="G166" s="4" t="s">
-        <v>484</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="G166" s="4"/>
       <c r="H166" s="4"/>
       <c r="I166" s="4"/>
       <c r="J166" s="4"/>
@@ -10004,24 +10019,26 @@
     </row>
     <row r="167" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>279</v>
+        <v>481</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>480</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>154</v>
+        <v>482</v>
       </c>
       <c r="E167" s="4" t="s">
         <v>355</v>
       </c>
       <c r="F167" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="G167" s="4"/>
+        <v>483</v>
+      </c>
+      <c r="G167" s="4" t="s">
+        <v>484</v>
+      </c>
       <c r="H167" s="4"/>
       <c r="I167" s="4"/>
       <c r="J167" s="4"/>
@@ -10046,27 +10063,25 @@
       <c r="AC167" s="4"/>
     </row>
     <row r="168" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A168" s="3" t="s">
-        <v>214</v>
+      <c r="A168" s="4" t="s">
+        <v>280</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="C168" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C168" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D168" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="E168" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="F168" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G168" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="D168" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E168" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="F168" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="G168" s="4"/>
       <c r="H168" s="4"/>
       <c r="I168" s="4"/>
       <c r="J168" s="4"/>
@@ -10091,25 +10106,27 @@
       <c r="AC168" s="4"/>
     </row>
     <row r="169" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A169" s="4" t="s">
-        <v>534</v>
-      </c>
-      <c r="B169" s="4" t="s">
-        <v>535</v>
-      </c>
-      <c r="C169" s="4" t="s">
+      <c r="A169" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="C169" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D169" s="4" t="s">
-        <v>454</v>
-      </c>
-      <c r="E169" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="F169" s="4" t="s">
-        <v>536</v>
-      </c>
-      <c r="G169" s="4"/>
+      <c r="D169" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G169" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="H169" s="4"/>
       <c r="I169" s="4"/>
       <c r="J169" s="4"/>
@@ -10134,27 +10151,25 @@
       <c r="AC169" s="4"/>
     </row>
     <row r="170" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A170" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B170" s="3" t="s">
-        <v>637</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="D170" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E170" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="F170" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="G170" s="3" t="s">
-        <v>136</v>
-      </c>
+      <c r="A170" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="C170" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D170" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="E170" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="F170" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="G170" s="4"/>
       <c r="H170" s="4"/>
       <c r="I170" s="4"/>
       <c r="J170" s="4"/>
@@ -10179,25 +10194,27 @@
       <c r="AC170" s="4"/>
     </row>
     <row r="171" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A171" s="4" t="s">
-        <v>633</v>
-      </c>
-      <c r="B171" s="4" t="s">
-        <v>634</v>
-      </c>
-      <c r="C171" s="4" t="s">
-        <v>261</v>
+      <c r="A171" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>447</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="F171" s="4" t="s">
-        <v>636</v>
-      </c>
-      <c r="G171" s="4"/>
+        <v>355</v>
+      </c>
+      <c r="F171" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G171" s="3" t="s">
+        <v>136</v>
+      </c>
       <c r="H171" s="4"/>
       <c r="I171" s="4"/>
       <c r="J171" s="4"/>
@@ -10223,26 +10240,24 @@
     </row>
     <row r="172" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
-        <v>606</v>
+        <v>633</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>415</v>
+        <v>634</v>
       </c>
       <c r="C172" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D172" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="E172" s="4" t="s">
+      <c r="D172" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E172" s="3" t="s">
         <v>342</v>
       </c>
       <c r="F172" s="4" t="s">
-        <v>605</v>
-      </c>
-      <c r="G172" s="4" t="s">
-        <v>604</v>
-      </c>
+        <v>636</v>
+      </c>
+      <c r="G172" s="4"/>
       <c r="H172" s="4"/>
       <c r="I172" s="4"/>
       <c r="J172" s="4"/>
@@ -10268,24 +10283,26 @@
     </row>
     <row r="173" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
-        <v>268</v>
+        <v>606</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>270</v>
+        <v>415</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="D173" s="4" t="s">
-        <v>207</v>
+        <v>603</v>
       </c>
       <c r="E173" s="4" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="F173" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="G173" s="4"/>
+        <v>605</v>
+      </c>
+      <c r="G173" s="4" t="s">
+        <v>604</v>
+      </c>
       <c r="H173" s="4"/>
       <c r="I173" s="4"/>
       <c r="J173" s="4"/>
@@ -10310,12 +10327,24 @@
       <c r="AC173" s="4"/>
     </row>
     <row r="174" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A174" s="4"/>
-      <c r="B174" s="4"/>
-      <c r="C174" s="4"/>
-      <c r="D174" s="4"/>
-      <c r="E174" s="4"/>
-      <c r="F174" s="4"/>
+      <c r="A174" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D174" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E174" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="F174" s="4" t="s">
+        <v>208</v>
+      </c>
       <c r="G174" s="4"/>
       <c r="H174" s="4"/>
       <c r="I174" s="4"/>

</xml_diff>